<commit_message>
Se realizo el primer carge de informacion. Historias de usuario en Excel, e imagenes
</commit_message>
<xml_diff>
--- a/huPresentacion.xlsx
+++ b/huPresentacion.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="174">
   <si>
     <t>IDENTIFICACIÓN</t>
   </si>
@@ -743,6 +743,9 @@
   <si>
     <t>Login</t>
   </si>
+  <si>
+    <t>crear-prov</t>
+  </si>
 </sst>
 </file>
 
@@ -751,11 +754,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -991,101 +1001,104 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1310,7 +1323,7 @@
   <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1320,7 +1333,7 @@
     <col min="3" max="3" width="75" style="11" customWidth="1"/>
     <col min="4" max="4" width="53.28515625" style="11" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
@@ -1491,7 +1504,7 @@
       <c r="B8" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="40" t="s">
         <v>92</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -1500,7 +1513,9 @@
       <c r="E8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="13"/>
+      <c r="F8" s="39" t="s">
+        <v>173</v>
+      </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
@@ -1863,7 +1878,9 @@
       <c r="E24" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="13"/>
+      <c r="F24" s="39" t="s">
+        <v>173</v>
+      </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
@@ -2054,7 +2071,9 @@
       <c r="E33" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="13"/>
+      <c r="F33" s="39" t="s">
+        <v>173</v>
+      </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
@@ -2490,9 +2509,12 @@
     <hyperlink ref="F31" r:id="rId3"/>
     <hyperlink ref="F40" r:id="rId4"/>
     <hyperlink ref="F47" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6"/>
+    <hyperlink ref="F24" r:id="rId7"/>
+    <hyperlink ref="F33" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId6"/>
+  <pageSetup orientation="landscape" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>